<commit_message>
updated to latest versions
</commit_message>
<xml_diff>
--- a/models/vagus-nerve/source/vagus-nerve.xlsx
+++ b/models/vagus-nerve/source/vagus-nerve.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="295">
   <si>
     <t>id</t>
   </si>
@@ -127,7 +127,7 @@
     <t>TUBE</t>
   </si>
   <si>
-    <t>vm_3, vm_9</t>
+    <t>mat-epineurium,mat-fld-endoneurial</t>
   </si>
   <si>
     <t>vagus-pre-skull</t>
@@ -331,7 +331,7 @@
     <t>CL:0000540</t>
   </si>
   <si>
-    <t>vm_1</t>
+    <t>mat-endoneurium</t>
   </si>
   <si>
     <t>endoneurium</t>
@@ -340,10 +340,10 @@
     <t>UBERON:0000123</t>
   </si>
   <si>
-    <t>vm_4, vm_6, vm_7</t>
-  </si>
-  <si>
-    <t>vm_2</t>
+    <t>mat-collagen-fibers,mat-lymphocyte,mat-fibroblasts</t>
+  </si>
+  <si>
+    <t>mat-perineurium</t>
   </si>
   <si>
     <t>perineurium</t>
@@ -352,184 +352,187 @@
     <t>UBERON:0000121</t>
   </si>
   <si>
+    <t>mat-fibroblasts</t>
+  </si>
+  <si>
+    <t>mat-epineurium</t>
+  </si>
+  <si>
+    <t>epineurium</t>
+  </si>
+  <si>
+    <t>UBERON:0000124</t>
+  </si>
+  <si>
+    <t>mat-conn-tiss</t>
+  </si>
+  <si>
+    <t>connective tissue</t>
+  </si>
+  <si>
+    <t>NCIT:C32367</t>
+  </si>
+  <si>
+    <t>vm_5</t>
+  </si>
+  <si>
+    <t>blood vessels</t>
+  </si>
+  <si>
+    <t>UBERON:0001981</t>
+  </si>
+  <si>
+    <t>mat-lymphocyte</t>
+  </si>
+  <si>
+    <t>lymphocyte</t>
+  </si>
+  <si>
+    <t>FMA:62863</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fibroblasts </t>
+  </si>
+  <si>
+    <t>FMA:63877</t>
+  </si>
+  <si>
+    <t>mat-collagen-fibers</t>
+  </si>
+  <si>
+    <t>collagen fibers</t>
+  </si>
+  <si>
+    <t>FMA:63891</t>
+  </si>
+  <si>
+    <t>mat-fld-endoneurial</t>
+  </si>
+  <si>
+    <t>endoneurial fluid</t>
+  </si>
+  <si>
+    <t>UBERON:0011893</t>
+  </si>
+  <si>
+    <t>vm_10</t>
+  </si>
+  <si>
+    <t>Blood</t>
+  </si>
+  <si>
+    <t>UBERON:0000178</t>
+  </si>
+  <si>
+    <t>vm_11</t>
+  </si>
+  <si>
+    <t>Aqueous solution</t>
+  </si>
+  <si>
+    <t>FMA:85815</t>
+  </si>
+  <si>
+    <t>vm_12, vm_13, vm_14, vm_15, vm_16, vm_17, vm_18, vm_19, vm_20, vm_21</t>
+  </si>
+  <si>
+    <t>vm_12</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>CHEBI:15377</t>
+  </si>
+  <si>
+    <t>vm_13</t>
+  </si>
+  <si>
+    <t>Sodium ion</t>
+  </si>
+  <si>
+    <t>CHEBI:29101</t>
+  </si>
+  <si>
+    <t>vm_14</t>
+  </si>
+  <si>
+    <t>Potassium ion</t>
+  </si>
+  <si>
+    <t>CHEBI:29103</t>
+  </si>
+  <si>
+    <t>vm_15</t>
+  </si>
+  <si>
+    <t>Calcium ion</t>
+  </si>
+  <si>
+    <t>CHEBI:29108</t>
+  </si>
+  <si>
+    <t>vm_16</t>
+  </si>
+  <si>
+    <t>Chloride ion</t>
+  </si>
+  <si>
+    <t>CHEBI:17996</t>
+  </si>
+  <si>
+    <t>vm_17</t>
+  </si>
+  <si>
+    <t>Hydrogen ion</t>
+  </si>
+  <si>
+    <t>CHEBI:24636</t>
+  </si>
+  <si>
+    <t>vm_18</t>
+  </si>
+  <si>
+    <t>Hydroxide ion</t>
+  </si>
+  <si>
+    <t>CHEBI:16234</t>
+  </si>
+  <si>
+    <t>vm_19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bicarbonate ion </t>
+  </si>
+  <si>
+    <t>CHEBI:17544</t>
+  </si>
+  <si>
+    <t>vm_20</t>
+  </si>
+  <si>
+    <t>Liquid</t>
+  </si>
+  <si>
+    <t>vm_21</t>
+  </si>
+  <si>
+    <t>Fluid</t>
+  </si>
+  <si>
+    <t>UBERON:0006314</t>
+  </si>
+  <si>
+    <t>vm_22</t>
+  </si>
+  <si>
+    <t>Wall of vessel</t>
+  </si>
+  <si>
+    <t>UBERON:0035965</t>
+  </si>
+  <si>
     <t>vm_4</t>
-  </si>
-  <si>
-    <t>vm_3</t>
-  </si>
-  <si>
-    <t>epineurium</t>
-  </si>
-  <si>
-    <t>UBERON:0000124</t>
-  </si>
-  <si>
-    <t>connective tissue</t>
-  </si>
-  <si>
-    <t>NCIT:C32367</t>
-  </si>
-  <si>
-    <t>vm_5</t>
-  </si>
-  <si>
-    <t>blood vessels</t>
-  </si>
-  <si>
-    <t>UBERON:0001981</t>
-  </si>
-  <si>
-    <t>vm_6</t>
-  </si>
-  <si>
-    <t>lymphocyte</t>
-  </si>
-  <si>
-    <t>FMA:62863</t>
-  </si>
-  <si>
-    <t>vm_7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fibroblasts </t>
-  </si>
-  <si>
-    <t>FMA:63877</t>
-  </si>
-  <si>
-    <t>vm_8</t>
-  </si>
-  <si>
-    <t>collagen fibers</t>
-  </si>
-  <si>
-    <t>FMA:63891</t>
-  </si>
-  <si>
-    <t>vm_9</t>
-  </si>
-  <si>
-    <t>endoneurial fluid</t>
-  </si>
-  <si>
-    <t>UBERON:0011893</t>
-  </si>
-  <si>
-    <t>vm_10</t>
-  </si>
-  <si>
-    <t>Blood</t>
-  </si>
-  <si>
-    <t>UBERON:0000178</t>
-  </si>
-  <si>
-    <t>vm_11</t>
-  </si>
-  <si>
-    <t>Aqueous solution</t>
-  </si>
-  <si>
-    <t>FMA:85815</t>
-  </si>
-  <si>
-    <t>vm_12, vm_13, vm_14, vm_15, vm_16, vm_17, vm_18, vm_19, vm_20, vm_21</t>
-  </si>
-  <si>
-    <t>vm_12</t>
-  </si>
-  <si>
-    <t>Water</t>
-  </si>
-  <si>
-    <t>CHEBI:15377</t>
-  </si>
-  <si>
-    <t>vm_13</t>
-  </si>
-  <si>
-    <t>Sodium ion</t>
-  </si>
-  <si>
-    <t>CHEBI:29101</t>
-  </si>
-  <si>
-    <t>vm_14</t>
-  </si>
-  <si>
-    <t>Potassium ion</t>
-  </si>
-  <si>
-    <t>CHEBI:29103</t>
-  </si>
-  <si>
-    <t>vm_15</t>
-  </si>
-  <si>
-    <t>Calcium ion</t>
-  </si>
-  <si>
-    <t>CHEBI:29108</t>
-  </si>
-  <si>
-    <t>vm_16</t>
-  </si>
-  <si>
-    <t>Chloride ion</t>
-  </si>
-  <si>
-    <t>CHEBI:17996</t>
-  </si>
-  <si>
-    <t>vm_17</t>
-  </si>
-  <si>
-    <t>Hydrogen ion</t>
-  </si>
-  <si>
-    <t>CHEBI:24636</t>
-  </si>
-  <si>
-    <t>vm_18</t>
-  </si>
-  <si>
-    <t>Hydroxide ion</t>
-  </si>
-  <si>
-    <t>CHEBI:16234</t>
-  </si>
-  <si>
-    <t>vm_19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bicarbonate ion </t>
-  </si>
-  <si>
-    <t>CHEBI:17544</t>
-  </si>
-  <si>
-    <t>vm_20</t>
-  </si>
-  <si>
-    <t>Liquid</t>
-  </si>
-  <si>
-    <t>vm_21</t>
-  </si>
-  <si>
-    <t>Fluid</t>
-  </si>
-  <si>
-    <t>UBERON:0006314</t>
-  </si>
-  <si>
-    <t>vm_22</t>
-  </si>
-  <si>
-    <t>Wall of vessel</t>
-  </si>
-  <si>
-    <t>UBERON:0035965</t>
   </si>
   <si>
     <t>vm_23</t>
@@ -938,7 +941,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="22">
+  <fonts count="19">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -986,25 +989,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <color rgb="FF000000"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color rgb="FF555555"/>
-      <name val="Arial"/>
-    </font>
+    <font/>
     <font>
       <b/>
       <sz val="9.0"/>
@@ -1079,7 +1064,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="68">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1119,6 +1104,9 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -1188,52 +1176,14 @@
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1279,43 +1229,40 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -1606,106 +1553,106 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="73" t="s">
-        <v>270</v>
-      </c>
-      <c r="B2" s="74" t="s">
+      <c r="A2" s="61" t="s">
         <v>271</v>
       </c>
+      <c r="B2" s="62" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="73" t="s">
-        <v>272</v>
-      </c>
-      <c r="B3" s="75" t="s">
+      <c r="A3" s="61" t="s">
         <v>273</v>
       </c>
+      <c r="B3" s="63" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="73" t="s">
-        <v>274</v>
-      </c>
-      <c r="B4" s="76" t="s">
+      <c r="A4" s="61" t="s">
         <v>275</v>
       </c>
+      <c r="B4" s="64" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="73" t="s">
-        <v>276</v>
-      </c>
-      <c r="B5" s="76" t="s">
+      <c r="A5" s="61" t="s">
         <v>277</v>
       </c>
+      <c r="B5" s="64" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="73" t="s">
-        <v>278</v>
-      </c>
-      <c r="B6" s="76" t="s">
+      <c r="A6" s="61" t="s">
         <v>279</v>
       </c>
+      <c r="B6" s="64" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="73" t="s">
-        <v>280</v>
-      </c>
-      <c r="B7" s="76" t="s">
+      <c r="A7" s="61" t="s">
         <v>281</v>
       </c>
+      <c r="B7" s="64" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="73" t="s">
-        <v>282</v>
-      </c>
-      <c r="B8" s="76" t="s">
+      <c r="A8" s="61" t="s">
         <v>283</v>
       </c>
+      <c r="B8" s="64" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="73" t="s">
-        <v>284</v>
-      </c>
-      <c r="B9" s="76" t="s">
+      <c r="A9" s="61" t="s">
         <v>285</v>
       </c>
+      <c r="B9" s="64" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="73" t="s">
-        <v>286</v>
-      </c>
-      <c r="B10" s="76" t="s">
+      <c r="A10" s="61" t="s">
         <v>287</v>
       </c>
+      <c r="B10" s="64" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="73" t="s">
-        <v>288</v>
-      </c>
-      <c r="B11" s="76" t="s">
+      <c r="A11" s="61" t="s">
         <v>289</v>
+      </c>
+      <c r="B11" s="64" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="B12" s="77" t="s">
         <v>291</v>
       </c>
+      <c r="B12" s="65" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="78" t="s">
-        <v>292</v>
-      </c>
-      <c r="B13" s="79" t="s">
+      <c r="A13" s="66" t="s">
         <v>293</v>
+      </c>
+      <c r="B13" s="67" t="s">
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -1839,24 +1786,24 @@
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
       <c r="L2" s="9"/>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="13" t="s">
         <v>25</v>
       </c>
       <c r="N2" s="12"/>
       <c r="O2" s="12"/>
-      <c r="P2" s="13"/>
+      <c r="P2" s="14"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
     </row>
     <row r="3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="17" t="s">
         <v>28</v>
       </c>
       <c r="E3" s="10" t="s">
@@ -1874,19 +1821,19 @@
       <c r="M3" s="12"/>
       <c r="N3" s="12"/>
       <c r="O3" s="12"/>
-      <c r="P3" s="13"/>
+      <c r="P3" s="14"/>
       <c r="Q3" s="12"/>
       <c r="R3" s="12"/>
       <c r="S3" s="12"/>
     </row>
     <row r="4">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="16"/>
+      <c r="C4" s="17"/>
       <c r="E4" s="10"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
@@ -1894,13 +1841,13 @@
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
-      <c r="L4" s="17" t="s">
+      <c r="L4" s="18" t="s">
         <v>21</v>
       </c>
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
       <c r="O4" s="12"/>
-      <c r="P4" s="13"/>
+      <c r="P4" s="14"/>
       <c r="Q4" s="12"/>
       <c r="R4" s="12"/>
       <c r="S4" s="12"/>
@@ -1909,10 +1856,10 @@
       <c r="A5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="17" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="8"/>
@@ -1929,19 +1876,19 @@
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
       <c r="O5" s="12"/>
-      <c r="P5" s="13"/>
+      <c r="P5" s="14"/>
       <c r="Q5" s="12"/>
       <c r="R5" s="12"/>
       <c r="S5" s="12"/>
     </row>
     <row r="6">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="15" t="s">
         <v>35</v>
       </c>
       <c r="D6" s="8"/>
@@ -1954,21 +1901,21 @@
       <c r="K6" s="12"/>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="20"/>
       <c r="Q6" s="12"/>
       <c r="R6" s="12"/>
       <c r="S6" s="12"/>
     </row>
     <row r="7">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="15" t="s">
         <v>38</v>
       </c>
       <c r="D7" s="8"/>
@@ -1982,20 +1929,20 @@
       <c r="L7" s="8"/>
       <c r="M7" s="12"/>
       <c r="N7" s="12"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="13"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="14"/>
       <c r="Q7" s="12"/>
       <c r="R7" s="12"/>
       <c r="S7" s="12"/>
     </row>
     <row r="8">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="15" t="s">
         <v>41</v>
       </c>
       <c r="D8" s="8"/>
@@ -2009,20 +1956,20 @@
       <c r="L8" s="8"/>
       <c r="M8" s="12"/>
       <c r="N8" s="12"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="13"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="14"/>
       <c r="Q8" s="12"/>
       <c r="R8" s="12"/>
       <c r="S8" s="12"/>
     </row>
     <row r="9">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="21" t="s">
         <v>44</v>
       </c>
       <c r="D9" s="8"/>
@@ -2038,20 +1985,20 @@
       </c>
       <c r="M9" s="12"/>
       <c r="N9" s="12"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="13"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="14"/>
       <c r="Q9" s="12"/>
       <c r="R9" s="12"/>
       <c r="S9" s="12"/>
     </row>
     <row r="10">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="15" t="s">
         <v>47</v>
       </c>
       <c r="D10" s="8"/>
@@ -2065,20 +2012,20 @@
       <c r="L10" s="8"/>
       <c r="M10" s="12"/>
       <c r="N10" s="12"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="13"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="14"/>
       <c r="Q10" s="12"/>
       <c r="R10" s="12"/>
       <c r="S10" s="12"/>
     </row>
     <row r="11">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="15" t="s">
         <v>50</v>
       </c>
       <c r="D11" s="8"/>
@@ -2093,55 +2040,55 @@
       <c r="M11" s="12"/>
       <c r="N11" s="12"/>
       <c r="O11" s="12"/>
-      <c r="P11" s="13"/>
+      <c r="P11" s="14"/>
       <c r="Q11" s="12"/>
       <c r="R11" s="12"/>
       <c r="S11" s="12"/>
     </row>
     <row r="12">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="22" t="s">
         <v>50</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="12"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="23" t="s">
         <v>53</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
-      <c r="L12" s="17" t="s">
+      <c r="L12" s="18" t="s">
         <v>21</v>
       </c>
       <c r="M12" s="12"/>
       <c r="N12" s="12"/>
       <c r="O12" s="12"/>
-      <c r="P12" s="13"/>
+      <c r="P12" s="14"/>
       <c r="Q12" s="12"/>
       <c r="R12" s="12"/>
       <c r="S12" s="12"/>
     </row>
     <row r="13">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="22" t="s">
         <v>50</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="12"/>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="23" t="s">
         <v>53</v>
       </c>
       <c r="G13" s="8"/>
@@ -2149,25 +2096,25 @@
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
-      <c r="L13" s="17" t="s">
+      <c r="L13" s="18" t="s">
         <v>21</v>
       </c>
       <c r="M13" s="12"/>
       <c r="N13" s="12"/>
       <c r="O13" s="12"/>
-      <c r="P13" s="13"/>
+      <c r="P13" s="14"/>
       <c r="Q13" s="12"/>
       <c r="R13" s="12"/>
       <c r="S13" s="12"/>
     </row>
     <row r="14">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="15" t="s">
         <v>58</v>
       </c>
       <c r="D14" s="8"/>
@@ -2182,19 +2129,19 @@
       <c r="M14" s="12"/>
       <c r="N14" s="12"/>
       <c r="O14" s="12"/>
-      <c r="P14" s="13"/>
+      <c r="P14" s="14"/>
       <c r="Q14" s="12"/>
       <c r="R14" s="12"/>
       <c r="S14" s="12"/>
     </row>
     <row r="15">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="15" t="s">
         <v>61</v>
       </c>
       <c r="D15" s="8"/>
@@ -2209,19 +2156,19 @@
       <c r="M15" s="12"/>
       <c r="N15" s="12"/>
       <c r="O15" s="12"/>
-      <c r="P15" s="13"/>
+      <c r="P15" s="14"/>
       <c r="Q15" s="12"/>
       <c r="R15" s="12"/>
       <c r="S15" s="12"/>
     </row>
     <row r="16">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="15" t="s">
         <v>64</v>
       </c>
       <c r="D16" s="8"/>
@@ -2236,19 +2183,19 @@
       <c r="M16" s="12"/>
       <c r="N16" s="12"/>
       <c r="O16" s="12"/>
-      <c r="P16" s="13"/>
+      <c r="P16" s="14"/>
       <c r="Q16" s="12"/>
       <c r="R16" s="12"/>
       <c r="S16" s="12"/>
     </row>
     <row r="17">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="15" t="s">
         <v>67</v>
       </c>
       <c r="D17" s="8"/>
@@ -2263,7 +2210,7 @@
       <c r="M17" s="12"/>
       <c r="N17" s="12"/>
       <c r="O17" s="12"/>
-      <c r="P17" s="19" t="s">
+      <c r="P17" s="20" t="s">
         <v>68</v>
       </c>
       <c r="Q17" s="12"/>
@@ -2271,13 +2218,13 @@
       <c r="S17" s="12"/>
     </row>
     <row r="18">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="15" t="s">
         <v>69</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="15" t="s">
         <v>71</v>
       </c>
       <c r="D18" s="8"/>
@@ -2292,19 +2239,19 @@
       <c r="M18" s="12"/>
       <c r="N18" s="12"/>
       <c r="O18" s="12"/>
-      <c r="P18" s="13"/>
+      <c r="P18" s="14"/>
       <c r="Q18" s="12"/>
       <c r="R18" s="12"/>
       <c r="S18" s="12"/>
     </row>
     <row r="19">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="24" t="s">
         <v>74</v>
       </c>
       <c r="D19" s="8"/>
@@ -2319,19 +2266,19 @@
       <c r="M19" s="12"/>
       <c r="N19" s="8"/>
       <c r="O19" s="8"/>
-      <c r="P19" s="13"/>
+      <c r="P19" s="14"/>
       <c r="Q19" s="12"/>
       <c r="R19" s="12"/>
       <c r="S19" s="12"/>
     </row>
     <row r="20">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="25" t="s">
         <v>77</v>
       </c>
       <c r="D20" s="8"/>
@@ -2348,77 +2295,77 @@
       <c r="M20" s="9"/>
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
-      <c r="P20" s="13"/>
+      <c r="P20" s="14"/>
       <c r="Q20" s="12"/>
       <c r="R20" s="12"/>
       <c r="S20" s="12"/>
     </row>
     <row r="21">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="D21" s="28"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="28" t="s">
+      <c r="D21" s="29"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="M21" s="29"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="30"/>
-      <c r="P21" s="31"/>
-      <c r="Q21" s="29"/>
-      <c r="R21" s="29"/>
-      <c r="S21" s="29"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="31"/>
+      <c r="O21" s="31"/>
+      <c r="P21" s="32"/>
+      <c r="Q21" s="30"/>
+      <c r="R21" s="30"/>
+      <c r="S21" s="30"/>
     </row>
     <row r="22">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="D22" s="28"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="28" t="s">
+      <c r="D22" s="29"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="M22" s="29"/>
-      <c r="N22" s="29"/>
-      <c r="O22" s="29"/>
-      <c r="P22" s="31"/>
-      <c r="Q22" s="29"/>
-      <c r="R22" s="29"/>
-      <c r="S22" s="29"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="30"/>
+      <c r="P22" s="32"/>
+      <c r="Q22" s="30"/>
+      <c r="R22" s="30"/>
+      <c r="S22" s="30"/>
     </row>
     <row r="23">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="21" t="s">
         <v>86</v>
       </c>
       <c r="D23" s="8"/>
@@ -2433,23 +2380,23 @@
       <c r="M23" s="12"/>
       <c r="N23" s="12"/>
       <c r="O23" s="12"/>
-      <c r="P23" s="13"/>
+      <c r="P23" s="14"/>
       <c r="Q23" s="12"/>
       <c r="R23" s="12"/>
       <c r="S23" s="12"/>
     </row>
     <row r="24">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="25" t="s">
         <v>89</v>
       </c>
       <c r="D24" s="9"/>
-      <c r="E24" s="32"/>
+      <c r="E24" s="33"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
@@ -2459,14 +2406,14 @@
       <c r="L24" s="9"/>
       <c r="M24" s="12"/>
       <c r="N24" s="12"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
+      <c r="O24" s="14"/>
+      <c r="P24" s="14"/>
       <c r="Q24" s="12"/>
       <c r="R24" s="12"/>
       <c r="S24" s="12"/>
     </row>
     <row r="25">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="14" t="s">
         <v>90</v>
       </c>
       <c r="B25" s="9" t="s">
@@ -2476,7 +2423,7 @@
         <v>92</v>
       </c>
       <c r="D25" s="9"/>
-      <c r="E25" s="32" t="b">
+      <c r="E25" s="33" t="b">
         <v>1</v>
       </c>
       <c r="F25" s="9"/>
@@ -2488,8 +2435,8 @@
       <c r="L25" s="9"/>
       <c r="M25" s="12"/>
       <c r="N25" s="12"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13"/>
+      <c r="O25" s="14"/>
+      <c r="P25" s="14"/>
       <c r="Q25" s="12"/>
       <c r="R25" s="12"/>
       <c r="S25" s="12"/>
@@ -2513,36 +2460,37 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="1" max="1" width="16.71"/>
     <col customWidth="1" min="2" max="2" width="20.86"/>
     <col customWidth="1" min="3" max="3" width="26.29"/>
-    <col customWidth="1" min="4" max="4" width="28.86"/>
+    <col customWidth="1" min="4" max="4" width="64.29"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="36" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="37" t="s">
         <v>93</v>
       </c>
       <c r="B2" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" t="s">
         <v>95</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="38" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2550,127 +2498,123 @@
       <c r="A3" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="38" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="D4" s="39" t="s">
-        <v>100</v>
+      <c r="D4" s="38" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="D7" s="37"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="D5" s="41"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="B6" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="D6" s="43"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="37" t="s">
-        <v>109</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="D7" s="44"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="D8" s="44"/>
+      <c r="D8" s="37"/>
     </row>
     <row r="9">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="37" t="s">
         <v>117</v>
       </c>
-      <c r="D9" s="44"/>
+      <c r="D9" s="37"/>
     </row>
     <row r="10">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="37" t="s">
         <v>119</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="37" t="s">
         <v>120</v>
       </c>
-      <c r="D10" s="44"/>
+      <c r="D10" s="37"/>
     </row>
     <row r="11">
       <c r="A11" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="D11" s="45" t="s">
-        <v>118</v>
-      </c>
+      <c r="D11" s="37"/>
     </row>
     <row r="12">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="37" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2678,171 +2622,161 @@
       <c r="A13" s="37" t="s">
         <v>128</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="D13" s="46"/>
     </row>
     <row r="14">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="D14" s="46"/>
     </row>
     <row r="15">
       <c r="A15" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="D15" s="46"/>
     </row>
     <row r="16">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="D16" s="46"/>
     </row>
     <row r="17">
       <c r="A17" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="37" t="s">
         <v>142</v>
       </c>
-      <c r="D17" s="46"/>
     </row>
     <row r="18">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="37" t="s">
         <v>143</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="37" t="s">
         <v>144</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="37" t="s">
         <v>145</v>
       </c>
-      <c r="D18" s="46"/>
     </row>
     <row r="19">
       <c r="A19" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="37" t="s">
         <v>147</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="D19" s="46"/>
     </row>
     <row r="20">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="37" t="s">
         <v>149</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="37" t="s">
         <v>150</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="D20" s="46"/>
     </row>
     <row r="21">
       <c r="A21" s="37" t="s">
         <v>152</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="37" t="s">
         <v>153</v>
       </c>
-      <c r="C21" s="47" t="s">
+      <c r="C21" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="D21" s="46"/>
     </row>
     <row r="22">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="37" t="s">
         <v>154</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="37" t="s">
         <v>155</v>
       </c>
-      <c r="C22" s="47" t="s">
+      <c r="C22" s="37" t="s">
         <v>156</v>
       </c>
-      <c r="D22" s="46"/>
     </row>
     <row r="23">
       <c r="A23" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="D23" s="44" t="s">
-        <v>100</v>
+      <c r="D23" s="37" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="37" t="s">
-        <v>160</v>
-      </c>
-      <c r="B24" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="C24" s="48" t="s">
+      <c r="B24" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="D24" s="44"/>
+      <c r="C24" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="D24" s="37"/>
     </row>
     <row r="25">
       <c r="A25" s="37" t="s">
-        <v>163</v>
-      </c>
-      <c r="B25" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="C25" s="48" t="s">
+      <c r="B25" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="D25" s="44"/>
+      <c r="C25" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="D25" s="37"/>
     </row>
     <row r="26">
-      <c r="A26" s="36" t="s">
-        <v>166</v>
-      </c>
-      <c r="B26" s="9" t="s">
+      <c r="A26" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="C26" s="49" t="s">
+      <c r="B26" s="37" t="s">
         <v>168</v>
       </c>
-      <c r="D26" s="44"/>
+      <c r="C26" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="D26" s="37"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2870,73 +2804,73 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="50" t="s">
-        <v>169</v>
-      </c>
-      <c r="D1" s="50" t="s">
+      <c r="C1" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="D1" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="E1" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="F1" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="50" t="s">
-        <v>172</v>
+      <c r="G1" s="39" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="B2" s="15"/>
+      <c r="A2" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="B2" s="16"/>
       <c r="C2" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D2" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="D2" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="E2" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="14"/>
+      <c r="F2" s="15"/>
       <c r="G2" s="12"/>
     </row>
     <row r="3">
-      <c r="A3" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="B3" s="15"/>
+      <c r="A3" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3" s="16"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="14"/>
+      <c r="F3" s="15"/>
       <c r="G3" s="12"/>
     </row>
     <row r="4">
-      <c r="A4" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="B4" s="15"/>
+      <c r="A4" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="B4" s="16"/>
       <c r="C4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="14" t="s">
+      <c r="D4" s="23"/>
+      <c r="E4" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="14"/>
+      <c r="F4" s="15"/>
       <c r="G4" s="12"/>
     </row>
   </sheetData>
@@ -2975,410 +2909,410 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="50" t="s">
-        <v>178</v>
-      </c>
-      <c r="E1" s="50" t="s">
+      <c r="D1" s="39" t="s">
         <v>179</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="E1" s="39" t="s">
         <v>180</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="F1" s="39" t="s">
         <v>181</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="G1" s="39" t="s">
+        <v>182</v>
+      </c>
+      <c r="H1" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="50" t="s">
-        <v>182</v>
-      </c>
-      <c r="J1" s="51" t="s">
+      <c r="I1" s="39" t="s">
         <v>183</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="J1" s="40" t="s">
         <v>184</v>
       </c>
-      <c r="L1" s="53" t="s">
+      <c r="K1" s="41" t="s">
         <v>185</v>
       </c>
-      <c r="M1" s="22" t="s">
-        <v>172</v>
+      <c r="L1" s="42" t="s">
+        <v>186</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="B2" s="15" t="s">
+      <c r="A2" s="15" t="s">
         <v>187</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>188</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="12"/>
-      <c r="E2" s="14">
+      <c r="E2" s="15">
         <v>229.0</v>
       </c>
-      <c r="F2" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="G2" s="22" t="s">
+      <c r="F2" s="23" t="s">
         <v>189</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>190</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
-      <c r="K2" s="54" t="s">
-        <v>190</v>
-      </c>
-      <c r="L2" s="14" t="s">
+      <c r="K2" s="43" t="s">
         <v>191</v>
       </c>
-      <c r="M2" s="55"/>
+      <c r="L2" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="M2" s="44"/>
     </row>
     <row r="3">
-      <c r="A3" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="B3" s="15" t="s">
+      <c r="A3" s="15" t="s">
         <v>193</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>194</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="12"/>
-      <c r="E3" s="14">
+      <c r="E3" s="15">
         <v>229.0</v>
       </c>
-      <c r="F3" s="22" t="s">
-        <v>194</v>
-      </c>
-      <c r="G3" s="22" t="s">
-        <v>189</v>
+      <c r="F3" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>190</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
-      <c r="K3" s="54" t="s">
-        <v>190</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>195</v>
+      <c r="K3" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>196</v>
       </c>
       <c r="M3" s="12"/>
     </row>
     <row r="4">
-      <c r="A4" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="B4" s="15" t="s">
+      <c r="A4" s="15" t="s">
         <v>197</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>198</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="12"/>
-      <c r="E4" s="14">
+      <c r="E4" s="15">
         <v>229.0</v>
       </c>
-      <c r="F4" s="22" t="s">
-        <v>198</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>189</v>
+      <c r="F4" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>190</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
-      <c r="K4" s="54" t="s">
-        <v>190</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="M4" s="55"/>
+      <c r="K4" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="M4" s="44"/>
     </row>
     <row r="5">
-      <c r="A5" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="B5" s="15" t="s">
+      <c r="A5" s="15" t="s">
         <v>201</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>202</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="12"/>
-      <c r="E5" s="14">
+      <c r="E5" s="15">
         <v>229.0</v>
       </c>
-      <c r="F5" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="G5" s="22" t="s">
-        <v>189</v>
+      <c r="F5" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>190</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
-      <c r="K5" s="54" t="s">
-        <v>190</v>
-      </c>
-      <c r="L5" s="14" t="s">
-        <v>203</v>
+      <c r="K5" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>204</v>
       </c>
       <c r="M5" s="12"/>
     </row>
     <row r="6">
-      <c r="A6" s="14" t="s">
-        <v>204</v>
-      </c>
-      <c r="B6" s="15" t="s">
+      <c r="A6" s="15" t="s">
         <v>205</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>206</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="12"/>
-      <c r="E6" s="14">
+      <c r="E6" s="15">
         <v>229.0</v>
       </c>
-      <c r="F6" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>206</v>
+      <c r="F6" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>207</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
-      <c r="K6" s="54" t="s">
-        <v>207</v>
-      </c>
-      <c r="L6" s="15" t="s">
+      <c r="K6" s="43" t="s">
         <v>208</v>
       </c>
+      <c r="L6" s="16" t="s">
+        <v>209</v>
+      </c>
       <c r="M6" s="12"/>
     </row>
     <row r="7">
-      <c r="A7" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="15" t="s">
         <v>210</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>211</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="12"/>
-      <c r="E7" s="14">
+      <c r="E7" s="15">
         <v>229.0</v>
       </c>
-      <c r="F7" s="22" t="s">
-        <v>206</v>
-      </c>
-      <c r="G7" s="22" t="s">
-        <v>211</v>
+      <c r="F7" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
-      <c r="K7" s="54" t="s">
-        <v>207</v>
-      </c>
-      <c r="L7" s="22" t="s">
-        <v>212</v>
+      <c r="K7" s="43" t="s">
+        <v>208</v>
+      </c>
+      <c r="L7" s="23" t="s">
+        <v>213</v>
       </c>
       <c r="M7" s="12"/>
     </row>
     <row r="8">
-      <c r="A8" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="B8" s="15" t="s">
+      <c r="A8" s="15" t="s">
         <v>214</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>215</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="12"/>
-      <c r="E8" s="14">
+      <c r="E8" s="15">
         <v>229.0</v>
       </c>
-      <c r="F8" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="G8" s="22" t="s">
+      <c r="F8" s="23" t="s">
         <v>216</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>217</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
-      <c r="K8" s="54" t="s">
-        <v>207</v>
-      </c>
-      <c r="L8" s="22" t="s">
-        <v>217</v>
+      <c r="K8" s="43" t="s">
+        <v>208</v>
+      </c>
+      <c r="L8" s="23" t="s">
+        <v>218</v>
       </c>
       <c r="M8" s="12"/>
     </row>
     <row r="9">
-      <c r="A9" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="B9" s="15" t="s">
+      <c r="A9" s="15" t="s">
         <v>219</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>220</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="12"/>
-      <c r="E9" s="14">
+      <c r="E9" s="15">
         <v>229.0</v>
       </c>
-      <c r="F9" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="G9" s="22" t="s">
+      <c r="F9" s="23" t="s">
         <v>221</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>222</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
-      <c r="K9" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="L9" s="14" t="s">
-        <v>222</v>
+      <c r="K9" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>223</v>
       </c>
       <c r="M9" s="12"/>
     </row>
     <row r="10">
-      <c r="A10" s="56" t="s">
-        <v>223</v>
-      </c>
-      <c r="B10" s="57" t="s">
+      <c r="A10" s="45" t="s">
         <v>224</v>
       </c>
-      <c r="C10" s="58" t="s">
+      <c r="B10" s="46" t="s">
+        <v>225</v>
+      </c>
+      <c r="C10" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="59"/>
-      <c r="E10" s="56">
+      <c r="D10" s="48"/>
+      <c r="E10" s="45">
         <v>229.0</v>
       </c>
-      <c r="F10" s="60" t="s">
-        <v>220</v>
-      </c>
-      <c r="G10" s="60" t="s">
-        <v>225</v>
-      </c>
-      <c r="H10" s="59"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="61" t="s">
-        <v>207</v>
-      </c>
-      <c r="L10" s="57" t="s">
+      <c r="F10" s="49" t="s">
+        <v>221</v>
+      </c>
+      <c r="G10" s="49" t="s">
         <v>226</v>
       </c>
-      <c r="M10" s="62"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="50" t="s">
+        <v>208</v>
+      </c>
+      <c r="L10" s="46" t="s">
+        <v>227</v>
+      </c>
+      <c r="M10" s="51"/>
     </row>
     <row r="11">
-      <c r="A11" s="56" t="s">
-        <v>227</v>
-      </c>
-      <c r="B11" s="63" t="s">
+      <c r="A11" s="45" t="s">
         <v>228</v>
       </c>
-      <c r="C11" s="58" t="s">
+      <c r="B11" s="52" t="s">
+        <v>229</v>
+      </c>
+      <c r="C11" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="62"/>
-      <c r="E11" s="56">
+      <c r="D11" s="51"/>
+      <c r="E11" s="45">
         <v>229.0</v>
       </c>
-      <c r="F11" s="60" t="s">
-        <v>220</v>
-      </c>
-      <c r="G11" s="60" t="s">
-        <v>229</v>
-      </c>
-      <c r="H11" s="64"/>
-      <c r="I11" s="62"/>
-      <c r="J11" s="62"/>
-      <c r="K11" s="61" t="s">
-        <v>207</v>
-      </c>
-      <c r="L11" s="57" t="s">
+      <c r="F11" s="49" t="s">
+        <v>221</v>
+      </c>
+      <c r="G11" s="49" t="s">
         <v>230</v>
       </c>
-      <c r="M11" s="62"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="50" t="s">
+        <v>208</v>
+      </c>
+      <c r="L11" s="46" t="s">
+        <v>231</v>
+      </c>
+      <c r="M11" s="51"/>
     </row>
     <row r="12">
-      <c r="A12" s="56" t="s">
-        <v>231</v>
-      </c>
-      <c r="B12" s="63" t="s">
+      <c r="A12" s="45" t="s">
         <v>232</v>
       </c>
-      <c r="C12" s="58" t="s">
+      <c r="B12" s="52" t="s">
+        <v>233</v>
+      </c>
+      <c r="C12" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="62"/>
-      <c r="E12" s="56">
+      <c r="D12" s="51"/>
+      <c r="E12" s="45">
         <v>229.0</v>
       </c>
-      <c r="F12" s="60" t="s">
-        <v>220</v>
-      </c>
-      <c r="G12" s="60" t="s">
-        <v>233</v>
-      </c>
-      <c r="H12" s="64"/>
-      <c r="I12" s="62"/>
-      <c r="J12" s="62"/>
-      <c r="K12" s="61" t="s">
-        <v>207</v>
-      </c>
-      <c r="L12" s="65" t="s">
+      <c r="F12" s="49" t="s">
+        <v>221</v>
+      </c>
+      <c r="G12" s="49" t="s">
         <v>234</v>
       </c>
-      <c r="M12" s="62"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="50" t="s">
+        <v>208</v>
+      </c>
+      <c r="L12" s="54" t="s">
+        <v>235</v>
+      </c>
+      <c r="M12" s="51"/>
     </row>
     <row r="13">
-      <c r="A13" s="14" t="s">
-        <v>235</v>
-      </c>
-      <c r="B13" s="15"/>
+      <c r="A13" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="B13" s="16"/>
       <c r="C13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="66" t="s">
-        <v>236</v>
-      </c>
-      <c r="E13" s="17" t="s">
+      <c r="D13" s="55" t="s">
+        <v>237</v>
+      </c>
+      <c r="E13" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="22" t="s">
-        <v>174</v>
-      </c>
-      <c r="G13" s="67"/>
+      <c r="F13" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="G13" s="13"/>
       <c r="H13" s="9"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
-      <c r="K13" s="54"/>
-      <c r="L13" s="20"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="21"/>
       <c r="M13" s="12"/>
     </row>
   </sheetData>
@@ -3404,20 +3338,20 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="50" t="s">
-        <v>237</v>
+      <c r="D1" s="39" t="s">
+        <v>238</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -3433,17 +3367,17 @@
       <c r="Q1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="19" t="s">
-        <v>239</v>
-      </c>
-      <c r="B2" s="22" t="s">
+      <c r="A2" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="B2" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="9"/>
-      <c r="E2" s="32"/>
+      <c r="E2" s="33"/>
       <c r="F2" s="9"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -3451,24 +3385,24 @@
       <c r="J2" s="9"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
       <c r="O2" s="12"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
     </row>
     <row r="3">
-      <c r="A3" s="19" t="s">
-        <v>215</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>241</v>
-      </c>
-      <c r="C3" s="16" t="s">
+      <c r="A3" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="9"/>
-      <c r="E3" s="32"/>
+      <c r="E3" s="33"/>
       <c r="F3" s="9"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -3476,21 +3410,21 @@
       <c r="J3" s="9"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
       <c r="O3" s="12"/>
       <c r="P3" s="12"/>
       <c r="Q3" s="12"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -3515,16 +3449,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2">
@@ -3532,24 +3466,24 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6">
@@ -3557,34 +3491,34 @@
         <v>0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -3611,43 +3545,43 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="68" t="s">
-        <v>178</v>
-      </c>
-      <c r="D1" s="68" t="s">
-        <v>259</v>
+      <c r="C1" s="56" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>260</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="G1" s="69" t="s">
-        <v>172</v>
+        <v>262</v>
+      </c>
+      <c r="G1" s="57" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="69" t="s">
         <v>264</v>
       </c>
+      <c r="C2" s="58"/>
+      <c r="D2" s="57" t="s">
+        <v>265</v>
+      </c>
       <c r="E2" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="G2" s="71"/>
+        <v>266</v>
+      </c>
+      <c r="G2" s="59"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -3669,17 +3603,17 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>